<commit_message>
Added the updated version of Supplemental Table 8.
</commit_message>
<xml_diff>
--- a/Analysis/Genomics_manuscript_TIR/Supplemental_Figures/Supplemental_Table_8.xlsx
+++ b/Analysis/Genomics_manuscript_TIR/Supplemental_Figures/Supplemental_Table_8.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work_Files\GCMP_TIR\immunity_microbiome\Supplemental_Figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F533EED5-19A3-4F93-A664-ABFB4EA167C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC87D4A-0691-4782-A1C4-DD10FD1EC69C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3132" yWindow="1908" windowWidth="17280" windowHeight="8964" xr2:uid="{1D9A66A8-7322-49B3-B858-11998F327895}"/>
+    <workbookView xWindow="3828" yWindow="2604" windowWidth="17280" windowHeight="8964" xr2:uid="{1D9A66A8-7322-49B3-B858-11998F327895}"/>
   </bookViews>
   <sheets>
     <sheet name="Table S8A" sheetId="1" r:id="rId1"/>
@@ -101,28 +101,28 @@
     <t>lm(y_trait_positive ~ x_trait_positive -1)</t>
   </si>
   <si>
-    <t>Phylogenetic comparison of IL-1R, and TLR gene family copies vs. Alpha Diversity in all compartments.</t>
-  </si>
-  <si>
-    <t>Phylogenetic comparison of IL-1R, and TLR gene family copies vs. Alpha Diversity in the mucus compartment.</t>
-  </si>
-  <si>
-    <t>Phylogenetic comparison of IL-1R, and TLR gene family copies vs. Alpha Diversity in the tissue compartment.</t>
-  </si>
-  <si>
-    <t>Phylogenetic comparison of IL-1R, and TLR gene family copies vs. Alpha Diversity in the skeleton compartment.</t>
-  </si>
-  <si>
-    <t>Table S8A</t>
-  </si>
-  <si>
-    <t>Table S8B</t>
-  </si>
-  <si>
-    <t>Table S8C</t>
-  </si>
-  <si>
-    <t>Table S8D</t>
+    <t>Table S8A: Phylogenetic comparison of IL-1R and TLR gene family copies vs Alpha Diversity in all compartments</t>
+  </si>
+  <si>
+    <t>Phylogenetic independent contranst results for IL-1R and TLR gene families for ln ASVs and Gini Index in all compartments combined for the coral microbiome data collected during the Global Coral Microbiome Project. All analyses were conducted using the phyloseq package in R. Outputs were also corrected for multiple comparisons by immune trait (eg IL-1R or TLR).</t>
+  </si>
+  <si>
+    <t>Table S8B: Phylogenetic comparison of IL-1R and TLR gene family copies vs. Alpha Diversity in the mucus compartment</t>
+  </si>
+  <si>
+    <t>Phylogenetic independent contranst results for IL-1R and TLR gene families for ln ASVs and Gini Index the mucus compartment combined for the coral microbiome data collected during the Global Coral Microbiome Project. All analyses were conducted using the phyloseq package in R. Outputs were also corrected for multiple comparisons by immune trait (eg IL-1R or TLR).</t>
+  </si>
+  <si>
+    <t>Table S8C: Phylogenetic comparison of IL-1R and TLR gene family copies vs. Alpha Diversity in the tissue compartment</t>
+  </si>
+  <si>
+    <t>Phylogenetic independent contranst results for IL-1R and TLR gene families for ln ASVs and Gini Index the tissue compartment combined for the coral microbiome data collected during the Global Coral Microbiome Project. All analyses were conducted using the phyloseq package in R. Outputs were also corrected for multiple comparisons by immune trait (eg IL-1R or TLR).</t>
+  </si>
+  <si>
+    <t>Table S8D: Phylogenetic comparison of IL-1R and TLR gene family copies vs Alpha Diversity in the skeleton compartment</t>
+  </si>
+  <si>
+    <t>Phylogenetic independent contranst results for IL-1R and TLR gene families for ln ASVs and Gini Index the skeleton compartment combined for the coral microbiome data collected during the Global Coral Microbiome Project. All analyses were conducted using the phyloseq package in R. Outputs were also corrected for multiple comparisons by immune trait (eg IL-1R or TLR).</t>
   </si>
 </sst>
 </file>
@@ -195,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -209,9 +209,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -530,7 +527,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A2" sqref="A2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -548,21 +545,31 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -726,8 +733,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -738,7 +745,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A2" sqref="A2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -754,23 +761,33 @@
     <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:10" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -934,8 +951,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -946,7 +963,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A2" sqref="A2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -964,21 +981,31 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="A2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1142,8 +1169,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1154,7 +1181,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1172,21 +1199,31 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
-    </row>
-    <row r="2" spans="1:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1350,8 +1387,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>